<commit_message>
preliminary results and plots
</commit_message>
<xml_diff>
--- a/Plotting/production_shares_ammonia_Scope1-3.xlsx
+++ b/Plotting/production_shares_ammonia_Scope1-3.xlsx
@@ -453,7 +453,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,6 +488,27 @@
       </c>
       <c r="I1" s="1" t="n"/>
       <c r="J1" s="1" t="n"/>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration_3</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="n"/>
+      <c r="M1" s="1" t="n"/>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration_4</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="n"/>
+      <c r="P1" s="1" t="n"/>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Iteration_5</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="n"/>
+      <c r="S1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -540,6 +561,51 @@
           <t>2050</t>
         </is>
       </c>
+      <c r="K2" s="1" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="L2" s="1" t="inlineStr">
+        <is>
+          <t>2040</t>
+        </is>
+      </c>
+      <c r="M2" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="N2" s="1" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="O2" s="1" t="inlineStr">
+        <is>
+          <t>2040</t>
+        </is>
+      </c>
+      <c r="P2" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
+      <c r="Q2" s="1" t="inlineStr">
+        <is>
+          <t>2030</t>
+        </is>
+      </c>
+      <c r="R2" s="1" t="inlineStr">
+        <is>
+          <t>2040</t>
+        </is>
+      </c>
+      <c r="S2" s="1" t="inlineStr">
+        <is>
+          <t>2050</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -574,6 +640,33 @@
       <c r="J4" t="n">
         <v>0</v>
       </c>
+      <c r="K4" t="n">
+        <v>35238095.23809672</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0</v>
+      </c>
+      <c r="N4" t="n">
+        <v>35238095.23810001</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>35238095.23809924</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -608,6 +701,33 @@
       <c r="J5" t="n">
         <v>0</v>
       </c>
+      <c r="K5" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -642,6 +762,33 @@
       <c r="J6" t="n">
         <v>27515499.01900796</v>
       </c>
+      <c r="K6" t="n">
+        <v>1.875326958742353e-06</v>
+      </c>
+      <c r="L6" t="n">
+        <v>21050082.96890682</v>
+      </c>
+      <c r="M6" t="n">
+        <v>27515499.01900796</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-2.29368470520229e-06</v>
+      </c>
+      <c r="O6" t="n">
+        <v>21030622.5940332</v>
+      </c>
+      <c r="P6" t="n">
+        <v>27515499.01900796</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>2.445282953989949e-06</v>
+      </c>
+      <c r="R6" t="n">
+        <v>21050125.12373882</v>
+      </c>
+      <c r="S6" t="n">
+        <v>27515499.0302716</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -676,6 +823,33 @@
       <c r="J7" t="n">
         <v>524945.5239729478</v>
       </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.001279717154111567</v>
+      </c>
+      <c r="M7" t="n">
+        <v>524944.0002144425</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.899009467186991e-06</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" t="n">
+        <v>524945.5253625842</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>1.775074794745918e-07</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-2.878535474074976e-05</v>
+      </c>
+      <c r="S7" t="n">
+        <v>524953.17614479</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -710,6 +884,33 @@
       <c r="J8" t="n">
         <v>0</v>
       </c>
+      <c r="K8" t="n">
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -744,6 +945,33 @@
       <c r="J9" t="n">
         <v>0</v>
       </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -778,6 +1006,33 @@
       <c r="J10" t="n">
         <v>0</v>
       </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -812,6 +1067,33 @@
       <c r="J11" t="n">
         <v>0</v>
       </c>
+      <c r="K11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -846,6 +1128,33 @@
       <c r="J12" t="n">
         <v>0</v>
       </c>
+      <c r="K12" t="n">
+        <v>0</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -880,6 +1189,33 @@
       <c r="J13" t="n">
         <v>0</v>
       </c>
+      <c r="K13" t="n">
+        <v>0</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -914,6 +1250,33 @@
       <c r="J14" t="n">
         <v>0</v>
       </c>
+      <c r="K14" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -948,12 +1311,42 @@
       <c r="J15" t="n">
         <v>0</v>
       </c>
+      <c r="K15" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>0</v>
+      </c>
+      <c r="P15" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>0</v>
+      </c>
+      <c r="R15" t="n">
+        <v>0</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="B1:D1"/>
+    <mergeCell ref="N1:P1"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="E1:G1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>